<commit_message>
added strategy probability method
</commit_message>
<xml_diff>
--- a/Axelrod FP.xlsx
+++ b/Axelrod FP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpaulmintz/Dissertation/Analysis (git)/Still-Falls Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB91A49E-70AB-734D-B976-7F6477FC6CD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944191CD-597F-3E41-9222-893B951D7C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2480" windowWidth="28040" windowHeight="16100" xr2:uid="{C5A99E80-ED8F-0C4D-90B9-C385916291CE}"/>
+    <workbookView xWindow="6340" yWindow="600" windowWidth="28040" windowHeight="15980" xr2:uid="{C5A99E80-ED8F-0C4D-90B9-C385916291CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,47 +510,17 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -904,7 +874,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -917,31 +887,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -983,13 +953,13 @@
       <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1036,13 +1006,13 @@
       <c r="N3" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="O3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1089,13 +1059,13 @@
       <c r="N4" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1142,13 +1112,13 @@
       <c r="N5" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1195,13 +1165,13 @@
       <c r="N6" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="2" t="s">
+      <c r="O6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1248,13 +1218,13 @@
       <c r="N7" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1301,13 +1271,13 @@
       <c r="N8" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1354,13 +1324,13 @@
       <c r="N9" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1407,13 +1377,13 @@
       <c r="N10" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="2" t="s">
+      <c r="P10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1460,13 +1430,13 @@
       <c r="N11" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1513,13 +1483,13 @@
       <c r="N12" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1566,13 +1536,13 @@
       <c r="N13" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1619,13 +1589,13 @@
       <c r="N14" t="s">
         <v>53</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1672,13 +1642,13 @@
       <c r="N15" t="s">
         <v>3</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1725,13 +1695,13 @@
       <c r="N16" t="s">
         <v>42</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1778,13 +1748,13 @@
       <c r="N17" t="s">
         <v>3</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="P17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1831,13 +1801,13 @@
       <c r="N18" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1884,13 +1854,13 @@
       <c r="N19" t="s">
         <v>39</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="O19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="P19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1937,13 +1907,13 @@
       <c r="N20" t="s">
         <v>3</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P20" s="2" t="s">
+      <c r="O20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="Q20" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1990,13 +1960,13 @@
       <c r="N21" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q21" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2043,13 +2013,13 @@
       <c r="N22" t="s">
         <v>3</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="2" t="s">
+      <c r="P22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2096,13 +2066,13 @@
       <c r="N23" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="P23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="Q23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2149,13 +2119,13 @@
       <c r="N24" t="s">
         <v>55</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2202,13 +2172,13 @@
       <c r="N25" t="s">
         <v>3</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="O25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="P25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2255,13 +2225,13 @@
       <c r="N26" t="s">
         <v>42</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2308,13 +2278,13 @@
       <c r="N27" t="s">
         <v>3</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q27" s="2" t="s">
+      <c r="O27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2361,13 +2331,13 @@
       <c r="N28" t="s">
         <v>3</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="O28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="P28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="Q28" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2414,13 +2384,13 @@
       <c r="N29" t="s">
         <v>46</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="O29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="P29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="Q29" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2467,22 +2437,22 @@
       <c r="N30" t="s">
         <v>42</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="O30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="P30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="Q30" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="F32" t="s">
         <v>139</v>
       </c>
@@ -2604,13 +2574,13 @@
       <c r="B40" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2730,13 +2700,13 @@
       <c r="B49" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2744,13 +2714,13 @@
       <c r="B50" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2898,24 +2868,24 @@
       <c r="B61" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <conditionalFormatting sqref="I3:K30">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unk">

</xml_diff>